<commit_message>
Making changes for testng reports
</commit_message>
<xml_diff>
--- a/MavenDummySelTest/Excel/POIdemo.xlsx
+++ b/MavenDummySelTest/Excel/POIdemo.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="86">
   <si>
     <t xml:space="preserve">RunMode</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>38108</t>
+  </si>
+  <si>
+    <t>83364</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
         <v>27</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>29</v>
@@ -681,7 +684,7 @@
         <v>45</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>29</v>
@@ -820,7 +823,7 @@
         <v>82</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
commiting changes related to testng.xml
</commit_message>
<xml_diff>
--- a/MavenDummySelTest/Excel/POIdemo.xlsx
+++ b/MavenDummySelTest/Excel/POIdemo.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="87">
   <si>
     <t xml:space="preserve">RunMode</t>
   </si>
@@ -281,6 +281,9 @@
   </si>
   <si>
     <t>83364</t>
+  </si>
+  <si>
+    <t>30876</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
@@ -499,7 +502,7 @@
         <v>27</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>29</v>
@@ -536,7 +539,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B7" activeCellId="0" pane="topLeft" sqref="B7"/>
@@ -583,7 +586,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
@@ -684,7 +687,7 @@
         <v>45</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>29</v>
@@ -721,7 +724,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="G1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="L2" activeCellId="0" pane="topLeft" sqref="L2"/>
@@ -823,7 +826,7 @@
         <v>82</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>29</v>

</xml_diff>